<commit_message>
Finished Breakdown per CMFID
</commit_message>
<xml_diff>
--- a/source/Databases/NxseSales/PAYROLL/REPORTS/PayPeriod -- 001.xlsx
+++ b/source/Databases/NxseSales/PAYROLL/REPORTS/PayPeriod -- 001.xlsx
@@ -5,15 +5,21 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CodeBaseSOS\NIMIS\source\Databases\NxseSales\PAYROLL\REPORTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\NIMIS\source\Databases\NxseSales\PAYROLL\REPORTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26310" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26310" windowHeight="12360"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="3091516" sheetId="2" r:id="rId2"/>
+    <sheet name="3091519" sheetId="3" r:id="rId3"/>
+    <sheet name="3091547" sheetId="4" r:id="rId4"/>
+    <sheet name="3091548" sheetId="5" r:id="rId5"/>
+    <sheet name="3091539" sheetId="6" r:id="rId6"/>
+    <sheet name="3091555" sheetId="7" r:id="rId7"/>
+    <sheet name="3091556" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="92">
   <si>
     <t>AccountID</t>
   </si>
@@ -207,9 +213,6 @@
     <t>EXCELLENT</t>
   </si>
   <si>
-    <t>travh001</t>
-  </si>
-  <si>
     <t>H Travlee II</t>
   </si>
   <si>
@@ -283,6 +286,27 @@
   </si>
   <si>
     <t>Total Pay</t>
+  </si>
+  <si>
+    <t>POINTSGIVEN</t>
+  </si>
+  <si>
+    <t>Points Given Away - Amount per point given</t>
+  </si>
+  <si>
+    <t>PMTCC</t>
+  </si>
+  <si>
+    <t>Payment Type - Credit Card</t>
+  </si>
+  <si>
+    <t>ACTWAIVED</t>
+  </si>
+  <si>
+    <t>Activation Fee - Waived</t>
+  </si>
+  <si>
+    <t>TRAVH001</t>
   </si>
 </sst>
 </file>
@@ -291,8 +315,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -332,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -366,30 +390,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -673,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,22 +760,22 @@
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
@@ -1384,16 +1421,16 @@
         <v>37</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>42</v>
@@ -1438,7 +1475,7 @@
         <v>60</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA6" s="2">
         <v>0</v>
@@ -1512,10 +1549,10 @@
         <v>37</v>
       </c>
       <c r="H7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>52</v>
@@ -1640,16 +1677,16 @@
         <v>37</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>42</v>
@@ -1755,8 +1792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,22 +1808,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1797,10 +1834,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="E2" s="7">
         <v>450</v>
@@ -1817,10 +1854,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="E3" s="7">
         <v>500</v>
@@ -1834,11 +1871,744 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D5" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="8">
+        <f>SUM(E2:E3)</f>
+        <v>950</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="7">
+        <v>450</v>
+      </c>
+      <c r="F2" s="10">
+        <v>42115.829507326387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="7">
+        <v>500</v>
+      </c>
+      <c r="F3" s="10">
+        <v>42115.829507372684</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E5" s="8">
+      <c r="D4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-165</v>
+      </c>
+      <c r="F4" s="10">
+        <v>42115.829348842592</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="8">
         <f>SUM(E2:E4)</f>
-        <v>950</v>
+        <v>785</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="7">
+        <v>-585</v>
+      </c>
+      <c r="F2" s="14">
+        <v>42115.829348842592</v>
+      </c>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="7">
+        <v>450</v>
+      </c>
+      <c r="F3" s="14">
+        <v>42115.829507372684</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="7">
+        <v>500</v>
+      </c>
+      <c r="F4" s="14">
+        <v>42115.829507372684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="8">
+        <f>SUM(E2:E4)</f>
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="7">
+        <v>450</v>
+      </c>
+      <c r="F2" s="14">
+        <v>42115.829507372684</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="7">
+        <v>500</v>
+      </c>
+      <c r="F3" s="14">
+        <v>42115.829507407405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-210</v>
+      </c>
+      <c r="F4" s="14">
+        <v>42115.829348842592</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="8">
+        <f>SUM(E2:E4)</f>
+        <v>740</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="7">
+        <v>-105</v>
+      </c>
+      <c r="F2" s="14">
+        <v>42115.829348842592</v>
+      </c>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="7">
+        <v>-50</v>
+      </c>
+      <c r="F3" s="14">
+        <v>42115.829348842592</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>23</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="7">
+        <v>450</v>
+      </c>
+      <c r="F4" s="14">
+        <v>42115.829507407405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="7">
+        <v>500</v>
+      </c>
+      <c r="F5" s="14">
+        <v>42115.829507407405</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="8">
+        <f>SUM(E2:E5)</f>
+        <v>795</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="7">
+        <v>450</v>
+      </c>
+      <c r="F2" s="14">
+        <v>42115.829507407405</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>26</v>
+      </c>
+      <c r="B3" s="2">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="7">
+        <v>500</v>
+      </c>
+      <c r="F3" s="14">
+        <v>42115.829507407405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="7">
+        <v>-50</v>
+      </c>
+      <c r="F4" s="14">
+        <v>42115.829348842592</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="7">
+        <v>-600</v>
+      </c>
+      <c r="F5" s="14">
+        <v>42115.829348842592</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="8">
+        <f>SUM(E2:E5)</f>
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="8">
+        <v>-450</v>
+      </c>
+      <c r="F2" s="13">
+        <v>42115.829348842592</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="8">
+        <v>450</v>
+      </c>
+      <c r="F3" s="13">
+        <v>42115.829507407405</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="8">
+        <v>500</v>
+      </c>
+      <c r="F4" s="13">
+        <v>42115.829507407405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="8">
+        <f>SUM(E2:E4)</f>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>